<commit_message>
Fixed some issues+intitial design for HDU&FW
</commit_message>
<xml_diff>
--- a/OPCODES.xlsx
+++ b/OPCODES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KIMO/Desktop/Harvard_Arch_Processor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BADB1930-A70F-F64D-9DDA-CD72D09CB13E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30328C1E-1FF4-3341-8A6D-E3B1B2924AD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="0" windowWidth="27200" windowHeight="15360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="180">
   <si>
     <t>0x000</t>
   </si>
@@ -219,9 +219,6 @@
     <t>shr src2</t>
   </si>
   <si>
-    <t>Reg-Imm-Sel/CarrySetter/SELECTOR</t>
-  </si>
-  <si>
     <t>0xX/0x00/0x0000</t>
   </si>
   <si>
@@ -309,36 +306,18 @@
     <t>sub 2</t>
   </si>
   <si>
-    <t>0xX/0x00/0x00/0xX/0xX/0x000/0x0</t>
-  </si>
-  <si>
     <t>0x1011</t>
   </si>
   <si>
     <t>pass src2</t>
   </si>
   <si>
-    <t>0x1/0x00/0x1011</t>
-  </si>
-  <si>
     <t>0x1/0x00/0x0101</t>
   </si>
   <si>
-    <t>Stack-DataSelector/WriteEnable/ReadEnable/Reg-Pc/pc-pc+1/Stack-add-sub/branch/Stall/Flush</t>
-  </si>
-  <si>
     <t>0xX/0x0/0x0/0xX/0xX/0x000/0x0/0x0/0x0</t>
   </si>
   <si>
-    <t>0x1/0x1/0x0/0x1/0xX/0x001/0x0/0x0/0x0</t>
-  </si>
-  <si>
-    <t>0x1/0x0/0x1/0xX/0xX/0x010/0x0/0x0/0x0</t>
-  </si>
-  <si>
-    <t>0x1/0x1/0x0/0x0/0x0/0x100/0x1/0x0/0x1</t>
-  </si>
-  <si>
     <t>0x1/0x0/0x1/0xX/0xX/0x011/0x1//0x0/0x1</t>
   </si>
   <si>
@@ -381,34 +360,211 @@
     <t>0x1/0x1/0x0</t>
   </si>
   <si>
-    <t>Reg-Mem-Selector/WriteSelector/src-dst-sel/Stall/Flush/INEN</t>
-  </si>
-  <si>
-    <t>0x0/0x00/0x0/0x0/0x0/0x1</t>
-  </si>
-  <si>
     <t>0x0/0x1/0x0</t>
   </si>
   <si>
     <t>0x0/0x0/0x0</t>
   </si>
   <si>
-    <t>0x0/0x00/0x0/0x0/0x0/0x0</t>
-  </si>
-  <si>
-    <t>0x0/0x01/0x0/0x0/0x0/0x0</t>
-  </si>
-  <si>
-    <t>0x0/0x10/0x0/0x0/0x0/0x0</t>
-  </si>
-  <si>
-    <t>0x0/0x01/0x1/0x0/0x0/0x0</t>
-  </si>
-  <si>
-    <t>0x1/0x00/0x0/0x0/0x0/0x0</t>
-  </si>
-  <si>
-    <t>0x1/0x00/0x0/0x1/0x1/0x0</t>
+    <t>0x1/0x00/0x0100</t>
+  </si>
+  <si>
+    <t>Carry Setter</t>
+  </si>
+  <si>
+    <t>doesn’t affect</t>
+  </si>
+  <si>
+    <t>sets Carry</t>
+  </si>
+  <si>
+    <t>clears carry</t>
+  </si>
+  <si>
+    <t>0x0/0x0/0x1/0xX/0xX/0x000/0x0/0x0/0x0</t>
+  </si>
+  <si>
+    <t>0x0/0x1/0x0/0x0/0xX/0x000/0x0/0x0/0x0</t>
+  </si>
+  <si>
+    <t>Reg-Mem-Selector/WriteSelector/src-dst-sel/Stall/Flush/INEN/RETS</t>
+  </si>
+  <si>
+    <t>0x0/0x00/0x0/0x0/0x0/0x0/0x0</t>
+  </si>
+  <si>
+    <t>0x0/0x01/0x0/0x0/0x0/0x0/0x0</t>
+  </si>
+  <si>
+    <t>0x0/0x00/0x0/0x0/0x0/0x1/0x0</t>
+  </si>
+  <si>
+    <t>0x0/0x10/0x0/0x0/0x0/0x0/0x0</t>
+  </si>
+  <si>
+    <t>0x0/0x01/0x1/0x0/0x0/0x0/0x0</t>
+  </si>
+  <si>
+    <t>0x1/0x00/0x0/0x0/0x0/0x0/0x1</t>
+  </si>
+  <si>
+    <t>0x1/0x00/0x0/0x1/0x1/0x0/0x1</t>
+  </si>
+  <si>
+    <t>0x1/0x01/0x0/0x0/0x0/0x0/0x0</t>
+  </si>
+  <si>
+    <t>fetcher</t>
+  </si>
+  <si>
+    <t>pc+1</t>
+  </si>
+  <si>
+    <t>pc+2</t>
+  </si>
+  <si>
+    <t>m[sp]</t>
+  </si>
+  <si>
+    <t>result from exc</t>
+  </si>
+  <si>
+    <t>0x1/0x1/0x0/0x1/0xX/0x010/0x0/0x0/0x0</t>
+  </si>
+  <si>
+    <t>Stack Control</t>
+  </si>
+  <si>
+    <t>first</t>
+  </si>
+  <si>
+    <t>second</t>
+  </si>
+  <si>
+    <t>0x0</t>
+  </si>
+  <si>
+    <t>0x1/0x0/0x1/0xX/0xX/0x001/0x0/0x0/0x0</t>
+  </si>
+  <si>
+    <t>Data-Stack-Selector/WriteEnable/ReadEnable/PC-Reg/pc-pc+1/Stack-add-sub/branch/Stall/Flush</t>
+  </si>
+  <si>
+    <t>0x1/0x1/0x0/0x0/0x1/0x100/0x1/0x0/0x1</t>
+  </si>
+  <si>
+    <t>Decoder</t>
+  </si>
+  <si>
+    <t>Rsrc1</t>
+  </si>
+  <si>
+    <t>Rdst</t>
+  </si>
+  <si>
+    <t>Read Enable (REGFILE)</t>
+  </si>
+  <si>
+    <t>disabled</t>
+  </si>
+  <si>
+    <t>enabled</t>
+  </si>
+  <si>
+    <t>OUT Enable</t>
+  </si>
+  <si>
+    <t>write on out port</t>
+  </si>
+  <si>
+    <t>don’t write on out port</t>
+  </si>
+  <si>
+    <t>Reg-Imm</t>
+  </si>
+  <si>
+    <t>Reg</t>
+  </si>
+  <si>
+    <t>Imm</t>
+  </si>
+  <si>
+    <t>Reg-Imm-Sel/CarrySetter/ALU SELECTOR</t>
+  </si>
+  <si>
+    <t>Data-Stack-selector</t>
+  </si>
+  <si>
+    <t>stack pointer</t>
+  </si>
+  <si>
+    <t>EA mem</t>
+  </si>
+  <si>
+    <t>Write enable (Memory)</t>
+  </si>
+  <si>
+    <t>enabeled</t>
+  </si>
+  <si>
+    <t>Read enable (Memory)</t>
+  </si>
+  <si>
+    <t>Pc-Reg</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>REG</t>
+  </si>
+  <si>
+    <t>PC-PC+1</t>
+  </si>
+  <si>
+    <t>Stall</t>
+  </si>
+  <si>
+    <t>Flush</t>
+  </si>
+  <si>
+    <t>don’t stall</t>
+  </si>
+  <si>
+    <t>don’t flush</t>
+  </si>
+  <si>
+    <t>branch</t>
+  </si>
+  <si>
+    <t>don’t branch</t>
+  </si>
+  <si>
+    <t>IN Enable</t>
+  </si>
+  <si>
+    <t>don’t take IN</t>
+  </si>
+  <si>
+    <t>take IN</t>
+  </si>
+  <si>
+    <t>Rets</t>
+  </si>
+  <si>
+    <t>not a ret</t>
+  </si>
+  <si>
+    <t>a ret</t>
+  </si>
+  <si>
+    <t>Write enable (Ref)</t>
+  </si>
+  <si>
+    <t>take first</t>
+  </si>
+  <si>
+    <t>take second</t>
   </si>
 </sst>
 </file>
@@ -485,7 +641,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -507,6 +663,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -791,13 +950,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="116" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
     <col min="3" max="3" width="25.6640625" customWidth="1"/>
     <col min="4" max="4" width="18.1640625" customWidth="1"/>
@@ -807,7 +967,7 @@
     <col min="8" max="8" width="43.83203125" customWidth="1"/>
     <col min="9" max="9" width="53.5" customWidth="1"/>
     <col min="10" max="10" width="85" customWidth="1"/>
-    <col min="11" max="11" width="52.83203125" customWidth="1"/>
+    <col min="11" max="11" width="63" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -833,16 +993,16 @@
         <v>53</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>64</v>
+        <v>154</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>99</v>
+        <v>140</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -860,16 +1020,16 @@
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="1" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -887,16 +1047,16 @@
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="1" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -914,16 +1074,16 @@
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="1" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -943,16 +1103,16 @@
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="1" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -972,16 +1132,16 @@
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="1" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -1001,16 +1161,16 @@
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="1" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -1030,16 +1190,16 @@
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="1" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -1061,13 +1221,13 @@
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="1" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>124</v>
@@ -1094,16 +1254,16 @@
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="1" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -1127,16 +1287,16 @@
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="1" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -1160,16 +1320,16 @@
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="1" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -1193,16 +1353,16 @@
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="1" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -1222,16 +1382,16 @@
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="1" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -1255,13 +1415,13 @@
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="1" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>125</v>
@@ -1288,13 +1448,13 @@
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="1" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>125</v>
@@ -1317,16 +1477,16 @@
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="1" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>101</v>
+        <v>134</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
@@ -1345,17 +1505,17 @@
         <v>40</v>
       </c>
       <c r="G18" s="6"/>
-      <c r="H18" s="1" t="s">
-        <v>117</v>
+      <c r="H18" s="7" t="s">
+        <v>112</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>102</v>
+        <v>139</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
@@ -1375,16 +1535,16 @@
       </c>
       <c r="G19" s="6"/>
       <c r="H19" s="1" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>103</v>
+        <v>141</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -1401,14 +1561,14 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="7" t="s">
-        <v>121</v>
+      <c r="H20" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>126</v>
@@ -1428,14 +1588,14 @@
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
-      <c r="H21" s="7" t="s">
-        <v>121</v>
+      <c r="H21" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>127</v>
@@ -1458,16 +1618,16 @@
       </c>
       <c r="G22" s="6"/>
       <c r="H22" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="K22" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
@@ -1487,16 +1647,16 @@
       </c>
       <c r="G23" s="6"/>
       <c r="H23" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="K23" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
@@ -1516,16 +1676,16 @@
       </c>
       <c r="G24" s="6"/>
       <c r="H24" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="K24" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
@@ -1545,16 +1705,16 @@
       </c>
       <c r="G25" s="6"/>
       <c r="H25" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="K25" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
@@ -1578,16 +1738,16 @@
         <v>42</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
@@ -1609,16 +1769,16 @@
         <v>42</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>48</v>
+        <v>96</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
@@ -1644,16 +1804,16 @@
         <v>44</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>48</v>
+        <v>112</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>48</v>
+        <v>113</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>48</v>
+        <v>118</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
@@ -1679,16 +1839,16 @@
         <v>44</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>48</v>
+        <v>111</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>48</v>
+        <v>119</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
@@ -1703,17 +1863,19 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
+      <c r="C31" s="8" t="s">
+        <v>114</v>
+      </c>
       <c r="D31" s="8"/>
       <c r="E31" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F31" s="8"/>
       <c r="G31" s="8" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="H31" s="8"/>
       <c r="I31" s="1"/>
@@ -1722,24 +1884,28 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
+      <c r="C32" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="E32" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
@@ -1752,19 +1918,23 @@
       <c r="B33" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
+      <c r="C33" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="E33" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>18</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
@@ -1777,19 +1947,23 @@
       <c r="B34" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
+      <c r="C34" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="E34" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
@@ -1800,21 +1974,25 @@
         <v>56</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
+        <v>71</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="E35" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
@@ -1827,16 +2005,18 @@
       <c r="B36" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
+      <c r="C36" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="D36" s="8"/>
       <c r="E36" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="H36" s="8"/>
       <c r="I36" s="1"/>
@@ -1848,17 +2028,23 @@
         <v>58</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
+        <v>78</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="F37" s="8"/>
       <c r="G37" s="1" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
@@ -1869,17 +2055,25 @@
         <v>59</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
+        <v>79</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>138</v>
+      </c>
       <c r="G38" s="1" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
@@ -1890,17 +2084,25 @@
         <v>60</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
+        <v>80</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="G39" s="1" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
@@ -1913,15 +2115,21 @@
       <c r="B40" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
+      <c r="C40" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="F40" s="8"/>
       <c r="G40" s="1" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
@@ -1932,14 +2140,22 @@
         <v>62</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
+        <v>81</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="D41" s="8"/>
+      <c r="E41" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="H41" s="8"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
@@ -1949,120 +2165,230 @@
         <v>63</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
+        <v>82</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>138</v>
+      </c>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
+        <v>93</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="F43" s="8"/>
+      <c r="G43" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
+      <c r="A44" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="B44" s="8"/>
+      <c r="C44" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D44" s="8"/>
+      <c r="E44" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G44" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="H44" s="8"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
+      <c r="A45" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>138</v>
+      </c>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
+      <c r="A46" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="F46" s="8"/>
+      <c r="G46" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
+      <c r="A47" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="B47" s="8"/>
+      <c r="C47" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D47" s="8"/>
+      <c r="E47" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="F47" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="G47" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="H47" s="8"/>
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
+      <c r="A48" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>138</v>
+      </c>
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
+      <c r="A49" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="F49" s="8"/>
+      <c r="G49" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
+      <c r="A50" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="D50" s="8"/>
+      <c r="E50" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>138</v>
+      </c>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
@@ -2070,12 +2396,24 @@
       <c r="K50" s="1"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
+      <c r="A51" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
@@ -2083,10 +2421,18 @@
       <c r="K51" s="1"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
+      <c r="A52" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
@@ -2096,8 +2442,10 @@
       <c r="K52" s="1"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
+      <c r="A53" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="B53" s="8"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
@@ -2109,8 +2457,12 @@
       <c r="K53" s="1"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
+      <c r="A54" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
@@ -2122,8 +2474,12 @@
       <c r="K54" s="1"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
+      <c r="A55" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
@@ -2135,8 +2491,12 @@
       <c r="K55" s="1"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
+      <c r="A56" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
@@ -2149,7 +2509,9 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
+      <c r="B57" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
@@ -2434,12 +2796,29 @@
       <c r="K78" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="22">
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="E40:F40"/>
     <mergeCell ref="A31:B31"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="E31:F31"/>
     <mergeCell ref="G31:H31"/>
     <mergeCell ref="G36:H36"/>
+    <mergeCell ref="C36:D36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
fixed an error with the IADD instruction
</commit_message>
<xml_diff>
--- a/OPCODES.xlsx
+++ b/OPCODES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KIMO/Desktop/Harvard_Arch_Processor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49175D11-1112-AF41-8546-E95EE8F5D989}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E05F042-C6EC-CF4F-B37C-7EEFE673CB35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="182">
   <si>
     <t>0x000</t>
   </si>
@@ -219,33 +219,12 @@
     <t>shr src2</t>
   </si>
   <si>
-    <t>0xX/0x00/0x0000</t>
-  </si>
-  <si>
-    <t>0xX/0x01/0x0000</t>
-  </si>
-  <si>
-    <t>0xX/0x10/0x0000</t>
-  </si>
-  <si>
-    <t>0x0/0x00/0x0001</t>
-  </si>
-  <si>
-    <t>0x0/0x00/0x0010</t>
-  </si>
-  <si>
     <t>deactivated</t>
   </si>
   <si>
-    <t>0x0/0x00/0x0011</t>
-  </si>
-  <si>
     <t>0x0011</t>
   </si>
   <si>
-    <t>0x0/0x00/0x0100</t>
-  </si>
-  <si>
     <t>ALU Selector</t>
   </si>
   <si>
@@ -258,9 +237,6 @@
     <t>0x10</t>
   </si>
   <si>
-    <t>0x0/0x00/0x0101</t>
-  </si>
-  <si>
     <t>0x0101</t>
   </si>
   <si>
@@ -276,21 +252,6 @@
     <t>0x1010</t>
   </si>
   <si>
-    <t>0x0/0x00/0x0110</t>
-  </si>
-  <si>
-    <t>0x0/0x00/0x0111</t>
-  </si>
-  <si>
-    <t>0x0/0x00/0x1000</t>
-  </si>
-  <si>
-    <t>0x0/0x00/0x1001</t>
-  </si>
-  <si>
-    <t>0x0/0x00/0x1010</t>
-  </si>
-  <si>
     <t>Stack-add-sub</t>
   </si>
   <si>
@@ -312,9 +273,6 @@
     <t>pass src2</t>
   </si>
   <si>
-    <t>0x1/0x00/0x0101</t>
-  </si>
-  <si>
     <t>0xX/0x0/0x0/0xX/0xX/0x000/0x0/0x0/0x0</t>
   </si>
   <si>
@@ -366,9 +324,6 @@
     <t>0x0/0x0/0x0</t>
   </si>
   <si>
-    <t>0x1/0x00/0x0100</t>
-  </si>
-  <si>
     <t>Carry Setter</t>
   </si>
   <si>
@@ -384,9 +339,6 @@
     <t>0x0/0x0/0x1/0xX/0xX/0x000/0x0/0x0/0x0</t>
   </si>
   <si>
-    <t>0x0/0x1/0x0/0x0/0xX/0x000/0x0/0x0/0x0</t>
-  </si>
-  <si>
     <t>Reg-Mem-Selector/WriteSelector/src-dst-sel/Stall/Flush/INEN/RETS</t>
   </si>
   <si>
@@ -480,9 +432,6 @@
     <t>Imm</t>
   </si>
   <si>
-    <t>Reg-Imm-Sel/CarrySetter/ALU SELECTOR</t>
-  </si>
-  <si>
     <t>Data-Stack-selector</t>
   </si>
   <si>
@@ -510,9 +459,6 @@
     <t>REG</t>
   </si>
   <si>
-    <t>PC-PC+1</t>
-  </si>
-  <si>
     <t>Stall</t>
   </si>
   <si>
@@ -568,6 +514,63 @@
   </si>
   <si>
     <t>0x0/0x11/0x0/0x0/0x0/0x0/0x0</t>
+  </si>
+  <si>
+    <t>0x0/0x1/0x0/0x01/0xX/0x000/0x0/0x0/0x0</t>
+  </si>
+  <si>
+    <t>PC+1-PC</t>
+  </si>
+  <si>
+    <t>PC+1</t>
+  </si>
+  <si>
+    <t>Reg-Imm-Sel2/Reg-Imm-Sel/CarrySetter/ALU SELECTOR</t>
+  </si>
+  <si>
+    <t>0x0/0xX/0x00/0x0000</t>
+  </si>
+  <si>
+    <t>0x0/0xX/0x01/0x0000</t>
+  </si>
+  <si>
+    <t>0x0/0xX/0x10/0x0000</t>
+  </si>
+  <si>
+    <t>0x0/0x0/0x00/0x0001</t>
+  </si>
+  <si>
+    <t>0x0/0x0/0x00/0x0010</t>
+  </si>
+  <si>
+    <t>0x0/0x0/0x00/0x0100</t>
+  </si>
+  <si>
+    <t>0x0/0x0/0x00/0x0101</t>
+  </si>
+  <si>
+    <t>0x0/0x0/0x00/0x0110</t>
+  </si>
+  <si>
+    <t>0x0/0x0/0x00/0x0111</t>
+  </si>
+  <si>
+    <t>0x0/0x0/0x00/0x1000</t>
+  </si>
+  <si>
+    <t>0x0/0x0/0x00/0x0011</t>
+  </si>
+  <si>
+    <t>0x0/0x0/0x00/0x1001</t>
+  </si>
+  <si>
+    <t>0x0/0x0/0x00/0x1010</t>
+  </si>
+  <si>
+    <t>0x0/0x1/0x00/0x0100</t>
+  </si>
+  <si>
+    <t>0x1/0x0/0x00/0x0101</t>
   </si>
 </sst>
 </file>
@@ -953,9 +956,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="116" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="116" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C47" sqref="C47:D47"/>
+      <selection pane="bottomLeft" activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -996,16 +999,16 @@
         <v>53</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>151</v>
+        <v>166</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -1023,16 +1026,16 @@
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="1" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>64</v>
+        <v>167</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -1050,16 +1053,16 @@
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="1" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>65</v>
+        <v>168</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -1077,16 +1080,16 @@
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="1" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>66</v>
+        <v>169</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -1106,16 +1109,16 @@
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="1" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>67</v>
+        <v>170</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -1135,16 +1138,16 @@
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="1" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>68</v>
+        <v>171</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -1164,16 +1167,16 @@
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="1" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>64</v>
+        <v>167</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -1193,16 +1196,16 @@
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="1" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>64</v>
+        <v>167</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -1224,16 +1227,16 @@
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="1" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>72</v>
+        <v>172</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>180</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -1257,16 +1260,16 @@
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="1" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>77</v>
+        <v>173</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -1290,16 +1293,16 @@
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="1" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>83</v>
+        <v>174</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -1323,16 +1326,16 @@
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="1" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>84</v>
+        <v>175</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -1356,16 +1359,16 @@
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="1" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>85</v>
+        <v>176</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -1385,16 +1388,16 @@
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="1" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>70</v>
+        <v>177</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -1418,16 +1421,16 @@
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="1" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>86</v>
+        <v>178</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -1451,16 +1454,16 @@
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="1" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>87</v>
+        <v>179</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -1480,16 +1483,16 @@
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="1" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>72</v>
+        <v>172</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
@@ -1509,16 +1512,16 @@
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="7" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>64</v>
+        <v>167</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
@@ -1538,16 +1541,16 @@
       </c>
       <c r="G19" s="6"/>
       <c r="H19" s="1" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>72</v>
+        <v>172</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -1565,16 +1568,16 @@
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
       <c r="H20" s="1" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>72</v>
+        <v>172</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
@@ -1592,16 +1595,16 @@
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K21" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
@@ -1621,16 +1624,16 @@
       </c>
       <c r="G22" s="6"/>
       <c r="H22" s="1" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>72</v>
+        <v>172</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
@@ -1650,16 +1653,16 @@
       </c>
       <c r="G23" s="6"/>
       <c r="H23" s="1" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>72</v>
+        <v>172</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
@@ -1679,16 +1682,16 @@
       </c>
       <c r="G24" s="6"/>
       <c r="H24" s="1" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>72</v>
+        <v>172</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
@@ -1708,16 +1711,16 @@
       </c>
       <c r="G25" s="6"/>
       <c r="H25" s="1" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>72</v>
+        <v>172</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
@@ -1741,16 +1744,16 @@
         <v>42</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>95</v>
+        <v>181</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
@@ -1772,16 +1775,16 @@
         <v>42</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>113</v>
+        <v>180</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
@@ -1807,16 +1810,16 @@
         <v>44</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>113</v>
+        <v>180</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
@@ -1842,16 +1845,16 @@
         <v>44</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>64</v>
+        <v>167</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>119</v>
+        <v>163</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
@@ -1866,19 +1869,19 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B31" s="9"/>
       <c r="C31" s="9" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="D31" s="9"/>
       <c r="E31" s="9" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="F31" s="9"/>
       <c r="G31" s="9" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="H31" s="9"/>
       <c r="I31" s="1"/>
@@ -1887,28 +1890,28 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
@@ -1922,22 +1925,22 @@
         <v>9</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>18</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
@@ -1951,22 +1954,22 @@
         <v>37</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
@@ -1977,25 +1980,25 @@
         <v>56</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
@@ -2009,17 +2012,17 @@
         <v>38</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="D36" s="9"/>
       <c r="E36" s="1" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="H36" s="9"/>
       <c r="I36" s="1"/>
@@ -2031,23 +2034,23 @@
         <v>58</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="F37" s="9"/>
       <c r="G37" s="1" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
@@ -2058,25 +2061,25 @@
         <v>59</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
@@ -2087,25 +2090,25 @@
         <v>60</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>48</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
@@ -2119,20 +2122,20 @@
         <v>39</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="F40" s="9"/>
       <c r="G40" s="1" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
@@ -2143,20 +2146,20 @@
         <v>62</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="D41" s="9"/>
       <c r="E41" s="1" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="G41" s="9" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="H41" s="9"/>
       <c r="I41" s="1"/>
@@ -2168,25 +2171,25 @@
         <v>63</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>48</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
@@ -2194,23 +2197,23 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>48</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="F43" s="9"/>
       <c r="G43" s="1" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>48</v>
@@ -2221,21 +2224,21 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="9" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="B44" s="9"/>
       <c r="C44" s="9" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="D44" s="9"/>
       <c r="E44" s="1" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="G44" s="9" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="H44" s="9"/>
       <c r="I44" s="1"/>
@@ -2244,28 +2247,28 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>48</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
@@ -2273,23 +2276,23 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>48</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="F46" s="9"/>
       <c r="G46" s="1" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>48</v>
@@ -2300,21 +2303,21 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="9" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="B47" s="9"/>
       <c r="C47" s="9" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="D47" s="9"/>
       <c r="E47" s="8" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="G47" s="9" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
       <c r="H47" s="9"/>
       <c r="I47" s="1"/>
@@ -2323,28 +2326,28 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>48</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>172</v>
+        <v>154</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
@@ -2352,23 +2355,23 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>48</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
       <c r="F49" s="9"/>
       <c r="G49" s="1" t="s">
-        <v>173</v>
+        <v>155</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>48</v>
@@ -2379,18 +2382,18 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="9" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B50" s="9"/>
       <c r="C50" s="9" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
       <c r="D50" s="9"/>
       <c r="E50" s="1" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
@@ -2400,19 +2403,19 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>48</v>
@@ -2425,13 +2428,13 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>48</v>
@@ -2446,7 +2449,7 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="9" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="B53" s="9"/>
       <c r="C53" s="1"/>
@@ -2461,10 +2464,10 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -2478,10 +2481,10 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
@@ -2495,10 +2498,10 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
@@ -2512,10 +2515,10 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
@@ -2802,17 +2805,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="E40:F40"/>
     <mergeCell ref="A53:B53"/>
     <mergeCell ref="G41:H41"/>
     <mergeCell ref="E43:F43"/>
@@ -2824,6 +2816,17 @@
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E49:F49"/>
     <mergeCell ref="G47:H47"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="C36:D36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
fixed op codes error
</commit_message>
<xml_diff>
--- a/OPCODES.xlsx
+++ b/OPCODES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KIMO/Desktop/Harvard_Arch_Processor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E05F042-C6EC-CF4F-B37C-7EEFE673CB35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EE0C475-2C2D-3C48-827C-F7A69FB881C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="181">
   <si>
     <t>0x000</t>
   </si>
@@ -154,9 +154,6 @@
   </si>
   <si>
     <t>XXXXXXXXXXXXXXXX</t>
-  </si>
-  <si>
-    <t>0x00011</t>
   </si>
   <si>
     <t>00XXXXXXXXXXXXXX</t>
@@ -956,9 +953,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="116" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" zoomScale="116" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -978,37 +975,37 @@
   <sheetData>
     <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="D1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="H1" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -1026,16 +1023,16 @@
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -1053,16 +1050,16 @@
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -1080,16 +1077,16 @@
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -1109,16 +1106,16 @@
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -1138,21 +1135,21 @@
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>1</v>
@@ -1167,16 +1164,16 @@
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -1196,16 +1193,16 @@
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -1227,16 +1224,16 @@
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -1260,16 +1257,16 @@
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -1293,16 +1290,16 @@
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -1326,16 +1323,16 @@
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -1359,16 +1356,16 @@
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -1388,16 +1385,16 @@
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -1421,16 +1418,16 @@
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -1454,16 +1451,16 @@
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -1483,16 +1480,16 @@
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
@@ -1512,16 +1509,16 @@
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
@@ -1529,7 +1526,7 @@
         <v>34</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>0</v>
@@ -1541,16 +1538,16 @@
       </c>
       <c r="G19" s="6"/>
       <c r="H19" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -1558,7 +1555,7 @@
         <v>35</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>18</v>
@@ -1568,16 +1565,16 @@
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
       <c r="H20" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
@@ -1585,7 +1582,7 @@
         <v>36</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>17</v>
@@ -1595,16 +1592,16 @@
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
@@ -1624,16 +1621,16 @@
       </c>
       <c r="G22" s="6"/>
       <c r="H22" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
@@ -1653,16 +1650,16 @@
       </c>
       <c r="G23" s="6"/>
       <c r="H23" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
@@ -1682,16 +1679,16 @@
       </c>
       <c r="G24" s="6"/>
       <c r="H24" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
@@ -1711,16 +1708,16 @@
       </c>
       <c r="G25" s="6"/>
       <c r="H25" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
@@ -1744,16 +1741,16 @@
         <v>42</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
@@ -1775,16 +1772,16 @@
         <v>42</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
@@ -1807,19 +1804,19 @@
         <v>40</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
@@ -1842,19 +1839,19 @@
         <v>40</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
@@ -1869,19 +1866,19 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B31" s="9"/>
       <c r="C31" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D31" s="9"/>
       <c r="E31" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F31" s="9"/>
       <c r="G31" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H31" s="9"/>
       <c r="I31" s="1"/>
@@ -1890,28 +1887,28 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
@@ -1919,28 +1916,28 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>18</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
@@ -1948,28 +1945,28 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
@@ -1977,28 +1974,28 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
@@ -2006,23 +2003,23 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D36" s="9"/>
       <c r="E36" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H36" s="9"/>
       <c r="I36" s="1"/>
@@ -2031,26 +2028,26 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F37" s="9"/>
       <c r="G37" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
@@ -2058,28 +2055,28 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
@@ -2087,28 +2084,28 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
@@ -2116,26 +2113,26 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F40" s="9"/>
       <c r="G40" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
@@ -2143,23 +2140,23 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D41" s="9"/>
       <c r="E41" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G41" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H41" s="9"/>
       <c r="I41" s="1"/>
@@ -2168,28 +2165,28 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
@@ -2197,26 +2194,26 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F43" s="9"/>
       <c r="G43" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
@@ -2224,21 +2221,21 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B44" s="9"/>
       <c r="C44" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D44" s="9"/>
       <c r="E44" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G44" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H44" s="9"/>
       <c r="I44" s="1"/>
@@ -2247,28 +2244,28 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
@@ -2276,26 +2273,26 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F46" s="9"/>
       <c r="G46" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
@@ -2303,21 +2300,21 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B47" s="9"/>
       <c r="C47" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D47" s="9"/>
       <c r="E47" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G47" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H47" s="9"/>
       <c r="I47" s="1"/>
@@ -2326,28 +2323,28 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
@@ -2355,26 +2352,26 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F49" s="9"/>
       <c r="G49" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
@@ -2382,18 +2379,18 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B50" s="9"/>
       <c r="C50" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D50" s="9"/>
       <c r="E50" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
@@ -2403,22 +2400,22 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
@@ -2428,16 +2425,16 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
@@ -2449,7 +2446,7 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B53" s="9"/>
       <c r="C53" s="1"/>
@@ -2464,10 +2461,10 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -2481,10 +2478,10 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
@@ -2498,10 +2495,10 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
@@ -2515,10 +2512,10 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
@@ -2805,6 +2802,17 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="E40:F40"/>
     <mergeCell ref="A53:B53"/>
     <mergeCell ref="G41:H41"/>
     <mergeCell ref="E43:F43"/>
@@ -2816,17 +2824,6 @@
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E49:F49"/>
     <mergeCell ref="G47:H47"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="C36:D36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
added remade design and controls after pahse 1
</commit_message>
<xml_diff>
--- a/OPCODES.xlsx
+++ b/OPCODES.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KIMO/Desktop/Harvard_Arch_Processor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A71D541C-439E-EB4C-A812-E2A6BED5D7D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50AB25E9-BB20-6643-9D9A-AC186D762535}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25600" yWindow="0" windowWidth="25600" windowHeight="14400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="2" r:id="rId1"/>
+    <sheet name="Updated Controls" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="293">
   <si>
     <t>0x000</t>
   </si>
@@ -604,13 +605,313 @@
   </si>
   <si>
     <t>Rets(INT1&amp;INT2)</t>
+  </si>
+  <si>
+    <t>ReadEnable/Rdst_Rsrc1/Rdst_Rsrc2</t>
+  </si>
+  <si>
+    <t>Result_Mem/WriteEnable/IN/MemPC_RegPC</t>
+  </si>
+  <si>
+    <t>0x0/0x00/0x0/0x0</t>
+  </si>
+  <si>
+    <t>ReadEnable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0 =&gt; disabled </t>
+  </si>
+  <si>
+    <t>0x1 =&gt; enabled</t>
+  </si>
+  <si>
+    <t>Rdst_Rsrc1</t>
+  </si>
+  <si>
+    <t>0x0 =&gt; Rdst</t>
+  </si>
+  <si>
+    <t>0x1 =&gt; Rsrc1</t>
+  </si>
+  <si>
+    <t>Rdst_Rsrc2</t>
+  </si>
+  <si>
+    <t>0x1 =&gt; Rsrc2</t>
+  </si>
+  <si>
+    <t>OUT</t>
+  </si>
+  <si>
+    <t>Branch</t>
+  </si>
+  <si>
+    <t>Set_Clr_Carry</t>
+  </si>
+  <si>
+    <t>0x00 =&gt; disabled</t>
+  </si>
+  <si>
+    <t>0x01 =&gt; set</t>
+  </si>
+  <si>
+    <t>0x10 =&gt; clear</t>
+  </si>
+  <si>
+    <t>0x11 =&gt; disabled</t>
+  </si>
+  <si>
+    <t>OUT/Branch/Set_Clr_Carry/Reg_IMM/PC_Reg/ALU_Selc</t>
+  </si>
+  <si>
+    <t>Reg_IMM</t>
+  </si>
+  <si>
+    <t>0x0 =&gt; Reg</t>
+  </si>
+  <si>
+    <t>0x1 =&gt; IMM</t>
+  </si>
+  <si>
+    <t>Push Flags</t>
+  </si>
+  <si>
+    <t>pop m[3] &amp; m[2]</t>
+  </si>
+  <si>
+    <t>push pc</t>
+  </si>
+  <si>
+    <t>reti</t>
+  </si>
+  <si>
+    <t>pop pc</t>
+  </si>
+  <si>
+    <t>pop flags</t>
+  </si>
+  <si>
+    <t>0x0 =&gt; Data</t>
+  </si>
+  <si>
+    <t>0x1 =&gt; Stack</t>
+  </si>
+  <si>
+    <t>0x0 =&gt; Result</t>
+  </si>
+  <si>
+    <t>SPSel</t>
+  </si>
+  <si>
+    <t>0x000 =&gt; disabled</t>
+  </si>
+  <si>
+    <t>0x0 =&gt; disabled</t>
+  </si>
+  <si>
+    <t>WriteEnable</t>
+  </si>
+  <si>
+    <t>Result_Mem</t>
+  </si>
+  <si>
+    <t>0x1 =&gt; MEM</t>
+  </si>
+  <si>
+    <t>0x01 =&gt; enable 1</t>
+  </si>
+  <si>
+    <t>0x10 =&gt; enable 1 &amp; 2</t>
+  </si>
+  <si>
+    <t>0x0 =&gt; RegPc</t>
+  </si>
+  <si>
+    <t>0x1 =&gt; MEMPC</t>
+  </si>
+  <si>
+    <t>0x1/0x0/0x0</t>
+  </si>
+  <si>
+    <t>PC_Reg</t>
+  </si>
+  <si>
+    <t>0x0 =&gt; PC</t>
+  </si>
+  <si>
+    <t>0x1 =&gt; Reg</t>
+  </si>
+  <si>
+    <t>ALU_Sel</t>
+  </si>
+  <si>
+    <t>0x0000 =&gt; disabled</t>
+  </si>
+  <si>
+    <t>0x0001 =&gt; increment</t>
+  </si>
+  <si>
+    <t>0x0/0x01/0x0/0x0</t>
+  </si>
+  <si>
+    <t>0x0010 =&gt; decrement</t>
+  </si>
+  <si>
+    <t>0x0/0x01/0x1/0x0</t>
+  </si>
+  <si>
+    <t>0x0011 =&gt; pass 1</t>
+  </si>
+  <si>
+    <t>0x0/0x10/0x0/0x0</t>
+  </si>
+  <si>
+    <t>0x0100 =&gt; Add 1 &amp; 2</t>
+  </si>
+  <si>
+    <t>0x0101 =&gt; Sub 1 &amp; 2</t>
+  </si>
+  <si>
+    <t>0x0110 =&gt; And 1 &amp; 2</t>
+  </si>
+  <si>
+    <t>0x0111 =&gt; Or 1 &amp; 2</t>
+  </si>
+  <si>
+    <t>Result_Mem/WriteEnable/IN/RegPC_MemPC</t>
+  </si>
+  <si>
+    <t>RegPC_MemPC</t>
+  </si>
+  <si>
+    <t>0x1000 =&gt; Not 1</t>
+  </si>
+  <si>
+    <t>0x1001 =&gt; SHL</t>
+  </si>
+  <si>
+    <t>0x1010 =&gt; SHR</t>
+  </si>
+  <si>
+    <t>Data_Stack</t>
+  </si>
+  <si>
+    <t>0x1/0x01/0x0/0x0</t>
+  </si>
+  <si>
+    <t>0x001 =&gt; push</t>
+  </si>
+  <si>
+    <t>0x1/0x00/0x0/0x1</t>
+  </si>
+  <si>
+    <t>Jmp/OUT/Branch/Set_Clr_Carry/Reg_IMM/PC_Reg/ALU_Selc</t>
+  </si>
+  <si>
+    <t>0x0/0x0/0x0/0x00/0x0/0x0/0x0000</t>
+  </si>
+  <si>
+    <t>0x0/0x0/0x0/0x01/0x0/0x0/0x0000</t>
+  </si>
+  <si>
+    <t>0x0/0x0/0x0/0x10/0x0/0x0/0x0000</t>
+  </si>
+  <si>
+    <t>0x0/0x0/0x0/0x00/0x0/0x1/0x0001</t>
+  </si>
+  <si>
+    <t>0x0/0x0/0x0/0x00/0x0/0x1/0x0010</t>
+  </si>
+  <si>
+    <t>0x0/0x1/0x0/0x00/0x0/0x0/0x0000</t>
+  </si>
+  <si>
+    <t>0x0/0x0/0x0/0x00/0x0/0x1/0x0100</t>
+  </si>
+  <si>
+    <t>0x0/0x0/0x0/0x00/0x0/0x1/0x0011</t>
+  </si>
+  <si>
+    <t>0x0/0x0/0x0/0x00/0x0/0x1/0x0101</t>
+  </si>
+  <si>
+    <t>0x0/0x0/0x0/0x00/0x0/0x1/0x0110</t>
+  </si>
+  <si>
+    <t>0x0/0x0/0x0/0x00/0x0/0x1/0x0111</t>
+  </si>
+  <si>
+    <t>0x0/0x0/0x0/0x00/0x0/0x1/0x1000</t>
+  </si>
+  <si>
+    <t>0x0/0x0/0x0/0x00/0x0/0x1/0x1001</t>
+  </si>
+  <si>
+    <t>0x0/0x0/0x0/0x00/0x0/0x1/0x1010</t>
+  </si>
+  <si>
+    <t>0x0/0x0/0x0/0x00/0x0/0x0/0x0001</t>
+  </si>
+  <si>
+    <t>0x0/0x0/0x1/0x00/0x0/0x0/0x0000</t>
+  </si>
+  <si>
+    <t>0x1/0x0/0x0/0x00/0x0/0x0/0x0000</t>
+  </si>
+  <si>
+    <t>0x0/0x0/0x0/0x00/0x1/0x1/0x0100</t>
+  </si>
+  <si>
+    <t>0x1011 =&gt; pass 2</t>
+  </si>
+  <si>
+    <t>0x0/0x0/0x0/0x00/0x1/0x1/0x1011</t>
+  </si>
+  <si>
+    <t>0x011 =&gt; call</t>
+  </si>
+  <si>
+    <t>0x010 =&gt; pop</t>
+  </si>
+  <si>
+    <t>0x100 =&gt; RET</t>
+  </si>
+  <si>
+    <t>Data_Stack/SPSel/ReadEnable/WriteEnable</t>
+  </si>
+  <si>
+    <t>Data_Stack/SPSel/ReadEnable/WriteEnable/Call/RETI</t>
+  </si>
+  <si>
+    <t>0x0/0x000/0x0/0x1/0x0/0x0</t>
+  </si>
+  <si>
+    <t>0x0/0x000/0x1/0x0/0x0/0x0</t>
+  </si>
+  <si>
+    <t>0x0/0x000/0x0/0x0/0x0/0x0</t>
+  </si>
+  <si>
+    <t>0x1/0x100/0x1/0x0/0x0/0x1</t>
+  </si>
+  <si>
+    <t>0x1/0x100/0x1/0x0/0x0/0x0</t>
+  </si>
+  <si>
+    <t>0x1/0x011/0x0/0x1/0x1/0x0</t>
+  </si>
+  <si>
+    <t>0x1/0x010/0x1/0x0/0x0/0x0</t>
+  </si>
+  <si>
+    <t>0x1/0x001/0x0/0x1/0x0/0x0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -641,8 +942,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -673,6 +1004,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5B9BD5"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -686,7 +1029,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -716,7 +1059,26 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1001,12 +1363,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="116" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G51" sqref="G51"/>
+    <sheetView zoomScale="50" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G29" sqref="A1:G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.1640625" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
@@ -1021,7 +1383,7 @@
     <col min="11" max="11" width="69.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="16">
       <c r="A1" s="4" t="s">
         <v>46</v>
       </c>
@@ -1056,7 +1418,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1083,7 +1445,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1110,7 +1472,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1137,7 +1499,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1166,7 +1528,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1195,7 +1557,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11">
       <c r="A7" s="1" t="s">
         <v>48</v>
       </c>
@@ -1224,7 +1586,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -1253,7 +1615,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -1284,7 +1646,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -1317,7 +1679,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -1350,7 +1712,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -1383,7 +1745,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -1416,7 +1778,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
@@ -1445,7 +1807,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -1478,7 +1840,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -1511,7 +1873,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11">
       <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
@@ -1540,7 +1902,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11">
       <c r="A18" s="1" t="s">
         <v>29</v>
       </c>
@@ -1569,7 +1931,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11">
       <c r="A19" s="1" t="s">
         <v>34</v>
       </c>
@@ -1598,7 +1960,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="16">
       <c r="A20" s="2" t="s">
         <v>35</v>
       </c>
@@ -1625,7 +1987,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11">
       <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
@@ -1652,7 +2014,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11">
       <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
@@ -1681,7 +2043,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11">
       <c r="A23" s="1" t="s">
         <v>31</v>
       </c>
@@ -1710,7 +2072,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11">
       <c r="A24" s="1" t="s">
         <v>32</v>
       </c>
@@ -1739,7 +2101,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11">
       <c r="A25" s="1" t="s">
         <v>33</v>
       </c>
@@ -1768,7 +2130,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -1801,7 +2163,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -1832,7 +2194,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
@@ -1867,7 +2229,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
@@ -1902,7 +2264,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1912,28 +2274,28 @@
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A31" s="9" t="s">
+    <row r="31" spans="1:11">
+      <c r="A31" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9" t="s">
+      <c r="B31" s="11"/>
+      <c r="C31" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9" t="s">
+      <c r="D31" s="11"/>
+      <c r="E31" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9" t="s">
+      <c r="F31" s="11"/>
+      <c r="G31" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="H31" s="9"/>
+      <c r="H31" s="11"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11">
       <c r="A32" s="1" t="s">
         <v>63</v>
       </c>
@@ -1962,7 +2324,7 @@
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11">
       <c r="A33" s="1" t="s">
         <v>53</v>
       </c>
@@ -1991,7 +2353,7 @@
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11">
       <c r="A34" s="1" t="s">
         <v>54</v>
       </c>
@@ -2020,7 +2382,7 @@
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11">
       <c r="A35" s="1" t="s">
         <v>55</v>
       </c>
@@ -2049,32 +2411,32 @@
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11">
       <c r="A36" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="9" t="s">
+      <c r="C36" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="D36" s="9"/>
+      <c r="D36" s="11"/>
       <c r="E36" s="1" t="s">
         <v>78</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G36" s="9" t="s">
+      <c r="G36" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="H36" s="9"/>
+      <c r="H36" s="11"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11">
       <c r="A37" s="1" t="s">
         <v>57</v>
       </c>
@@ -2087,10 +2449,10 @@
       <c r="D37" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E37" s="9" t="s">
+      <c r="E37" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="F37" s="9"/>
+      <c r="F37" s="11"/>
       <c r="G37" s="1" t="s">
         <v>86</v>
       </c>
@@ -2101,7 +2463,7 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11">
       <c r="A38" s="1" t="s">
         <v>58</v>
       </c>
@@ -2130,7 +2492,7 @@
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11">
       <c r="A39" s="1" t="s">
         <v>59</v>
       </c>
@@ -2159,7 +2521,7 @@
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11">
       <c r="A40" s="1" t="s">
         <v>60</v>
       </c>
@@ -2172,10 +2534,10 @@
       <c r="D40" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E40" s="9" t="s">
+      <c r="E40" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="F40" s="9"/>
+      <c r="F40" s="11"/>
       <c r="G40" s="1" t="s">
         <v>86</v>
       </c>
@@ -2186,32 +2548,32 @@
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11">
       <c r="A41" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C41" s="9" t="s">
+      <c r="C41" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="D41" s="9"/>
+      <c r="D41" s="11"/>
       <c r="E41" s="1" t="s">
         <v>117</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="G41" s="9" t="s">
+      <c r="G41" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="H41" s="9"/>
+      <c r="H41" s="11"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11">
       <c r="A42" s="1" t="s">
         <v>62</v>
       </c>
@@ -2240,7 +2602,7 @@
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11">
       <c r="A43" s="1" t="s">
         <v>80</v>
       </c>
@@ -2253,10 +2615,10 @@
       <c r="D43" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E43" s="9" t="s">
+      <c r="E43" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="F43" s="9"/>
+      <c r="F43" s="11"/>
       <c r="G43" s="1" t="s">
         <v>123</v>
       </c>
@@ -2267,30 +2629,30 @@
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A44" s="9" t="s">
+    <row r="44" spans="1:11">
+      <c r="A44" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="B44" s="9"/>
-      <c r="C44" s="9" t="s">
+      <c r="B44" s="11"/>
+      <c r="C44" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="D44" s="9"/>
+      <c r="D44" s="11"/>
       <c r="E44" s="1" t="s">
         <v>121</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="G44" s="9" t="s">
+      <c r="G44" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="H44" s="9"/>
+      <c r="H44" s="11"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11">
       <c r="A45" s="1" t="s">
         <v>108</v>
       </c>
@@ -2319,7 +2681,7 @@
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11">
       <c r="A46" s="1" t="s">
         <v>109</v>
       </c>
@@ -2332,10 +2694,10 @@
       <c r="D46" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E46" s="9" t="s">
+      <c r="E46" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="F46" s="9"/>
+      <c r="F46" s="11"/>
       <c r="G46" s="1" t="s">
         <v>123</v>
       </c>
@@ -2346,30 +2708,30 @@
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A47" s="9" t="s">
+    <row r="47" spans="1:11">
+      <c r="A47" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="B47" s="9"/>
-      <c r="C47" s="9" t="s">
+      <c r="B47" s="11"/>
+      <c r="C47" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="D47" s="9"/>
+      <c r="D47" s="11"/>
       <c r="E47" s="8" t="s">
         <v>131</v>
       </c>
       <c r="F47" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="G47" s="9" t="s">
+      <c r="G47" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="H47" s="9"/>
+      <c r="H47" s="11"/>
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11">
       <c r="A48" s="1" t="s">
         <v>126</v>
       </c>
@@ -2398,7 +2760,7 @@
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11">
       <c r="A49" s="1" t="s">
         <v>127</v>
       </c>
@@ -2411,10 +2773,10 @@
       <c r="D49" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E49" s="9" t="s">
+      <c r="E49" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="F49" s="9"/>
+      <c r="F49" s="11"/>
       <c r="G49" s="1" t="s">
         <v>138</v>
       </c>
@@ -2425,15 +2787,15 @@
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A50" s="9" t="s">
+    <row r="50" spans="1:11">
+      <c r="A50" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="B50" s="9"/>
-      <c r="C50" s="9" t="s">
+      <c r="B50" s="11"/>
+      <c r="C50" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="D50" s="9"/>
+      <c r="D50" s="11"/>
       <c r="E50" s="1" t="s">
         <v>136</v>
       </c>
@@ -2446,7 +2808,7 @@
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11">
       <c r="A51" s="1" t="s">
         <v>145</v>
       </c>
@@ -2471,7 +2833,7 @@
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11">
       <c r="A52" s="1" t="s">
         <v>126</v>
       </c>
@@ -2492,24 +2854,24 @@
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A53" s="9" t="s">
+    <row r="53" spans="1:11">
+      <c r="A53" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="B53" s="9"/>
-      <c r="C53" s="10" t="s">
+      <c r="B53" s="11"/>
+      <c r="C53" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="D53" s="10"/>
-      <c r="E53" s="10"/>
-      <c r="F53" s="10"/>
-      <c r="G53" s="10"/>
-      <c r="H53" s="11"/>
+      <c r="D53" s="12"/>
+      <c r="E53" s="12"/>
+      <c r="F53" s="12"/>
+      <c r="G53" s="12"/>
+      <c r="H53" s="10"/>
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11">
       <c r="A54" s="1" t="s">
         <v>111</v>
       </c>
@@ -2537,7 +2899,7 @@
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11">
       <c r="A55" s="1" t="s">
         <v>140</v>
       </c>
@@ -2566,7 +2928,7 @@
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11">
       <c r="A56" s="1" t="s">
         <v>141</v>
       </c>
@@ -2595,7 +2957,7 @@
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11">
       <c r="A57" s="1" t="s">
         <v>143</v>
       </c>
@@ -2624,7 +2986,7 @@
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1" t="s">
@@ -2649,7 +3011,7 @@
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -2662,7 +3024,7 @@
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -2675,7 +3037,7 @@
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -2688,7 +3050,7 @@
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -2701,7 +3063,7 @@
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -2714,7 +3076,7 @@
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -2727,7 +3089,7 @@
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -2740,7 +3102,7 @@
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -2753,7 +3115,7 @@
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -2766,7 +3128,7 @@
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -2779,7 +3141,7 @@
       <c r="J68" s="1"/>
       <c r="K68" s="1"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2792,7 +3154,7 @@
       <c r="J69" s="1"/>
       <c r="K69" s="1"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2805,7 +3167,7 @@
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -2818,7 +3180,7 @@
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -2831,7 +3193,7 @@
       <c r="J72" s="1"/>
       <c r="K72" s="1"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -2844,7 +3206,7 @@
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -2857,7 +3219,7 @@
       <c r="J74" s="1"/>
       <c r="K74" s="1"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -2870,7 +3232,7 @@
       <c r="J75" s="1"/>
       <c r="K75" s="1"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -2883,7 +3245,7 @@
       <c r="J76" s="1"/>
       <c r="K76" s="1"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -2896,7 +3258,7 @@
       <c r="J77" s="1"/>
       <c r="K77" s="1"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -2911,17 +3273,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="E40:F40"/>
     <mergeCell ref="A53:B53"/>
     <mergeCell ref="G41:H41"/>
     <mergeCell ref="E43:F43"/>
@@ -2934,8 +3285,1285 @@
     <mergeCell ref="E49:F49"/>
     <mergeCell ref="G47:H47"/>
     <mergeCell ref="C53:G53"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="C36:D36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C95019F-4CA9-094F-B57A-F55F25E7DD75}">
+  <dimension ref="A1:K63"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="57" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="B39" sqref="B39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="26.83203125" customWidth="1"/>
+    <col min="2" max="2" width="36.1640625" customWidth="1"/>
+    <col min="3" max="3" width="35.6640625" customWidth="1"/>
+    <col min="4" max="4" width="26.1640625" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" customWidth="1"/>
+    <col min="7" max="7" width="33.6640625" customWidth="1"/>
+    <col min="8" max="8" width="42.83203125" customWidth="1"/>
+    <col min="9" max="9" width="56" customWidth="1"/>
+    <col min="10" max="10" width="64.83203125" customWidth="1"/>
+    <col min="11" max="11" width="56.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="16">
+      <c r="A1" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="16"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="16"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="17"/>
+      <c r="H5" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="17"/>
+      <c r="H6" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="16"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="17"/>
+      <c r="H7" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="16"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="17"/>
+      <c r="H8" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="17"/>
+      <c r="F9" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="17"/>
+      <c r="H9" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="17"/>
+      <c r="H10" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="17"/>
+      <c r="H11" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="17"/>
+      <c r="H12" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="17"/>
+      <c r="H13" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="17"/>
+      <c r="H14" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" s="17"/>
+      <c r="H15" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" s="17"/>
+      <c r="H16" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G17" s="17"/>
+      <c r="H17" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G18" s="17"/>
+      <c r="H18" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G19" s="17"/>
+      <c r="H19" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="16">
+      <c r="A20" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G22" s="17"/>
+      <c r="H22" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G23" s="17"/>
+      <c r="H23" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G24" s="17"/>
+      <c r="H24" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G25" s="17"/>
+      <c r="H25" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26" s="17"/>
+      <c r="F26" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G27" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G28" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G29" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="K29" s="1"/>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+    </row>
+    <row r="33" spans="1:11" ht="16">
+      <c r="H33" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="I33" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="J33" s="14" t="s">
+        <v>283</v>
+      </c>
+      <c r="K33" s="14" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" t="s">
+        <v>182</v>
+      </c>
+      <c r="B34" t="s">
+        <v>218</v>
+      </c>
+      <c r="H34" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="I34" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="J34" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="K34" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" t="s">
+        <v>215</v>
+      </c>
+      <c r="B35" t="s">
+        <v>219</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="I35" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36" t="s">
+        <v>216</v>
+      </c>
+      <c r="B36" t="s">
+        <v>220</v>
+      </c>
+      <c r="H36" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="I36" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" t="s">
+        <v>217</v>
+      </c>
+      <c r="H37" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="I37" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="J37" s="9"/>
+      <c r="K37" s="9" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="H38" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="I38" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="H39" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="I39" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="H40" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="I40" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="J40" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="H41" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="H42" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="K42" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="H43" s="1"/>
+      <c r="I43" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="H44" s="1"/>
+      <c r="I44" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="H45" s="1"/>
+      <c r="I45" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="K45" s="9" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="H46" s="1"/>
+      <c r="I46" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="H47" s="1"/>
+      <c r="I47" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="H48" s="1"/>
+      <c r="I48" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
+    </row>
+    <row r="49" spans="8:11">
+      <c r="H49" s="1"/>
+      <c r="I49" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="J49" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="K49" s="1"/>
+    </row>
+    <row r="50" spans="8:11">
+      <c r="H50" s="1"/>
+      <c r="I50" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="K50" s="1"/>
+    </row>
+    <row r="51" spans="8:11">
+      <c r="H51" s="1"/>
+      <c r="I51" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="K51" s="1"/>
+    </row>
+    <row r="52" spans="8:11">
+      <c r="H52" s="1"/>
+      <c r="I52" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="J52" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="K52" s="1"/>
+    </row>
+    <row r="53" spans="8:11">
+      <c r="H53" s="1"/>
+      <c r="I53" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="K53" s="1"/>
+    </row>
+    <row r="54" spans="8:11">
+      <c r="H54" s="1"/>
+      <c r="I54" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="K54" s="1"/>
+    </row>
+    <row r="55" spans="8:11">
+      <c r="H55" s="1"/>
+      <c r="I55" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="J55" s="1"/>
+      <c r="K55" s="1"/>
+    </row>
+    <row r="56" spans="8:11">
+      <c r="H56" s="1"/>
+      <c r="I56" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="J56" s="1"/>
+      <c r="K56" s="1"/>
+    </row>
+    <row r="57" spans="8:11">
+      <c r="H57" s="1"/>
+      <c r="I57" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="J57" s="1"/>
+      <c r="K57" s="1"/>
+    </row>
+    <row r="58" spans="8:11">
+      <c r="H58" s="1"/>
+      <c r="I58" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="J58" s="1"/>
+      <c r="K58" s="1"/>
+    </row>
+    <row r="59" spans="8:11">
+      <c r="H59" s="1"/>
+      <c r="I59" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="J59" s="1"/>
+      <c r="K59" s="1"/>
+    </row>
+    <row r="60" spans="8:11">
+      <c r="I60" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="61" spans="8:11">
+      <c r="I61" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="62" spans="8:11">
+      <c r="I62" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="63" spans="8:11">
+      <c r="I63" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>